<commit_message>
Covered most of the requirements for date parsing
</commit_message>
<xml_diff>
--- a/date-js/timesheet.xlsx
+++ b/date-js/timesheet.xlsx
@@ -38,7 +38,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -99,7 +99,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -406,7 +406,7 @@
   <dimension ref="A4:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,22 +441,27 @@
         <v>41204</v>
       </c>
       <c r="B5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2">
         <f>SUM(B5:B24)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E5" s="2">
         <v>50</v>
       </c>
       <c r="F5" s="2">
         <f>D5*E5</f>
-        <v>50</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3">
+        <v>41205</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>

</xml_diff>

<commit_message>
Added culture info for mdy and dmy formats
</commit_message>
<xml_diff>
--- a/date-js/timesheet.xlsx
+++ b/date-js/timesheet.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A4:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,14 +445,14 @@
       </c>
       <c r="D5" s="2">
         <f>SUM(B5:B24)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E5" s="2">
         <v>50</v>
       </c>
       <c r="F5" s="2">
         <f>D5*E5</f>
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -460,7 +460,7 @@
         <v>41205</v>
       </c>
       <c r="B6" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added unit testing / fixed parsing bugs / todo: still need to fix unit tests failing...
</commit_message>
<xml_diff>
--- a/date-js/timesheet.xlsx
+++ b/date-js/timesheet.xlsx
@@ -445,14 +445,14 @@
       </c>
       <c r="D5" s="2">
         <f>SUM(B5:B24)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2">
         <v>50</v>
       </c>
       <c r="F5" s="2">
         <f>D5*E5</f>
-        <v>300</v>
+        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -464,7 +464,12 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="3">
+        <v>41206</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>

</xml_diff>

<commit_message>
Fixed parsing errors / unit tests
</commit_message>
<xml_diff>
--- a/date-js/timesheet.xlsx
+++ b/date-js/timesheet.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A4:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,14 +445,14 @@
       </c>
       <c r="D5" s="2">
         <f>SUM(B5:B24)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2">
         <v>50</v>
       </c>
       <c r="F5" s="2">
         <f>D5*E5</f>
-        <v>600</v>
+        <v>750</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -472,7 +472,12 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="3">
+        <v>41207</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>

</xml_diff>

<commit_message>
Fixed unit tests and added new parse expressions
</commit_message>
<xml_diff>
--- a/date-js/timesheet.xlsx
+++ b/date-js/timesheet.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A4:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,14 +445,14 @@
       </c>
       <c r="D5" s="2">
         <f>SUM(B5:B24)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
         <v>50</v>
       </c>
       <c r="F5" s="2">
         <f>D5*E5</f>
-        <v>750</v>
+        <v>800</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -480,7 +480,12 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="3">
+        <v>41208</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>

</xml_diff>